<commit_message>
Finished logic of cook and waiter
</commit_message>
<xml_diff>
--- a/init.xlsx
+++ b/init.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23200" yWindow="0" windowWidth="15200" windowHeight="21600" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="23200" yWindow="0" windowWidth="15200" windowHeight="21600" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Password" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>username</t>
   </si>
@@ -149,27 +149,18 @@
     <t>blob</t>
   </si>
   <si>
-    <t>peking0</t>
-  </si>
-  <si>
     <t>varchar(20)</t>
   </si>
   <si>
     <t>orderNo</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>totalPrice</t>
   </si>
   <si>
     <t>status</t>
   </si>
   <si>
-    <t>varchar(10)</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
@@ -213,6 +204,15 @@
   </si>
   <si>
     <t>Good!</t>
+  </si>
+  <si>
+    <t>ordertime</t>
+  </si>
+  <si>
+    <t>cookfoodtime</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,7 +908,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -917,7 +917,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>36</v>
@@ -925,16 +925,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +957,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
@@ -966,38 +966,38 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1012,7 +1012,7 @@
         <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1036,13 +1036,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1053,18 +1053,18 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1074,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,37 +1085,55 @@
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9">
         <v>43445.504166666666</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished waiter side adding customer
</commit_message>
<xml_diff>
--- a/init.xlsx
+++ b/init.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23200" yWindow="0" windowWidth="15200" windowHeight="21600" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Password" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,6 @@
     <sheet name="Order" sheetId="6" r:id="rId6"/>
     <sheet name="Comment" sheetId="7" r:id="rId7"/>
     <sheet name="CookFood" sheetId="8" r:id="rId8"/>
-    <sheet name="Include" sheetId="9" r:id="rId9"/>
-    <sheet name="Mention" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>username</t>
   </si>
@@ -149,9 +147,6 @@
     <t>blob</t>
   </si>
   <si>
-    <t>varchar(20)</t>
-  </si>
-  <si>
     <t>orderNo</t>
   </si>
   <si>
@@ -173,16 +168,10 @@
     <t>IN</t>
   </si>
   <si>
-    <t>commentNo</t>
-  </si>
-  <si>
     <t>content</t>
   </si>
   <si>
     <t>clob</t>
-  </si>
-  <si>
-    <t>comment0</t>
   </si>
   <si>
     <t>感觉很一般，菜品有点凉，不推荐</t>
@@ -219,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -276,6 +265,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -300,9 +297,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -316,7 +316,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -695,26 +698,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,7 +799,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,7 +868,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,7 +897,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -917,7 +906,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>36</v>
@@ -925,16 +914,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -947,7 +936,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +946,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
@@ -966,13 +955,13 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -986,18 +975,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1012,7 +1001,7 @@
         <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +1014,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,13 +1025,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1053,22 +1042,23 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1077,7 +1067,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1090,27 +1080,27 @@
         <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>4</v>
@@ -1121,7 +1111,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1130,25 +1120,13 @@
         <v>43445.504166666666</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>